<commit_message>
- poszerzone story i dashboardy - polaczenie mapy swiata i krajow - zmiany w tabeli zbiorczej
</commit_message>
<xml_diff>
--- a/Countries_Final_PL_14.xlsx
+++ b/Countries_Final_PL_14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matso\Desktop\Corona_tableau\Corona_tableau_rep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8DB606-79E7-4C7A-AA38-077E64307A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D25F89-19F2-4351-B0EE-0BC98DC6684D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2506" uniqueCount="1166">
   <si>
     <t>Continent</t>
   </si>
@@ -3586,6 +3586,12 @@
   </si>
   <si>
     <t>Statek "MS Zaandam"</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Sahara Zachodnia</t>
   </si>
 </sst>
 </file>
@@ -21089,10 +21095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H223"/>
+  <dimension ref="A1:H224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K219" sqref="K219"/>
+      <selection activeCell="A227" sqref="A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26218,6 +26224,29 @@
       </c>
       <c r="F223" s="11">
         <v>1829</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>2</v>
+      </c>
+      <c r="B224" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C224" s="9" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D224" s="9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E224" s="11">
+        <v>266000</v>
+      </c>
+      <c r="F224" s="11">
+        <v>567402</v>
+      </c>
+      <c r="G224" s="11">
+        <v>2.0299999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>